<commit_message>
fix: Adventurer keyId 'ADT'로 변경
</commit_message>
<xml_diff>
--- a/public/question-data.xlsx
+++ b/public/question-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Root\Desktop\test\SEAL-project\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2DA2590-52A5-4184-9C46-2795417E0E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C4C439-4FCC-4941-8780-26C1B8149C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="142">
   <si>
     <t>keyId</t>
   </si>
@@ -469,6 +469,18 @@
   </si>
   <si>
     <t>isPositive</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADT1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADT2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADT3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -850,8 +862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1388,7 +1400,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>14</v>
+        <v>139</v>
       </c>
       <c r="B29" t="s">
         <v>76</v>
@@ -1408,7 +1420,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>15</v>
+        <v>140</v>
       </c>
       <c r="B30" t="s">
         <v>76</v>
@@ -1428,7 +1440,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>16</v>
+        <v>141</v>
       </c>
       <c r="B31" t="s">
         <v>76</v>

</xml_diff>